<commit_message>
06-Fix delete selection and add duplicate check
</commit_message>
<xml_diff>
--- a/databases/DataBase_domiciliation.xlsx
+++ b/databases/DataBase_domiciliation.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA28"/>
+  <dimension ref="A1:AA27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -573,7 +573,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SKY NEST</t>
+          <t>HANINE INOX</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3338405000024</v>
+        <v>3480837000022</v>
       </c>
       <c r="D2" t="n">
         <v>100000</v>
@@ -597,47 +597,25 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°8</t>
-        </is>
-      </c>
+          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>Monsieur</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>Nawfal</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>ADERGHAL</t>
-        </is>
-      </c>
-      <c r="L2" t="n">
-        <v>29820</v>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Khemisset</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>Rue Addamir El Kabir Etg 04 Apt 32</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>X230258</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Associé Unique Gérant</t>
-        </is>
-      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
       <c r="T2" t="inlineStr">
         <is>
           <t>Casablanca</t>
@@ -646,16 +624,17 @@
       <c r="U2" t="n">
         <v>12</v>
       </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>1000 HT</t>
-        </is>
-      </c>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SKY MA</t>
+          <t>MARC PRISTIGE</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -664,7 +643,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3386797000030</v>
+        <v>3463115000015</v>
       </c>
       <c r="D3" t="n">
         <v>100000</v>
@@ -679,29 +658,25 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°9</t>
-        </is>
-      </c>
+          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°11</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr">
         <is>
           <t>Monsieur</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>SAMRI</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>RAZIK</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Associé Unique Gérant</t>
-        </is>
-      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr">
         <is>
           <t>Casablanca</t>
@@ -710,11 +685,17 @@
       <c r="U3" t="n">
         <v>12</v>
       </c>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>HANINE INOX</t>
+          <t>MAROFLEET</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -723,7 +704,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3480837000022</v>
+        <v>3458423000017</v>
       </c>
       <c r="D4" t="n">
         <v>100000</v>
@@ -738,14 +719,25 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
-        </is>
-      </c>
+          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°12</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr">
         <is>
           <t>Monsieur</t>
         </is>
       </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr">
         <is>
           <t>Casablanca</t>
@@ -754,11 +746,17 @@
       <c r="U4" t="n">
         <v>12</v>
       </c>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MARC PRISTIGE</t>
+          <t>ELBI LINK</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -767,7 +765,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3463115000015</v>
+        <v>3487719000060</v>
       </c>
       <c r="D5" t="n">
         <v>100000</v>
@@ -782,7 +780,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°11</t>
+          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>15-03-2024</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -790,6 +793,46 @@
           <t>Monsieur</t>
         </is>
       </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>AZIZ</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>QASBAJI</t>
+        </is>
+      </c>
+      <c r="L5" t="n">
+        <v>27346</v>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>RABAT</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>LOT ZAHRA NR 388 HAD SOUALEM BERRECHID</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>A781595</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>24-03-2029</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Associé Unique Gérant</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr">
         <is>
           <t>Casablanca</t>
@@ -798,23 +841,47 @@
       <c r="U5" t="n">
         <v>12</v>
       </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>19-03-2024</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>18-03-2025</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>19-03-2024</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>1000 HT</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MAROFLEET</t>
+          <t>LES NOUVEAUX BATISSEURS HAOUZ</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3458423000017</v>
-      </c>
-      <c r="D6" t="n">
-        <v>100000</v>
+        <v>3506233000023</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>100 000</t>
+        </is>
       </c>
       <c r="E6" t="n">
         <v>1000</v>
@@ -826,7 +893,12 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°12</t>
+          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>22-04-2024</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -834,19 +906,83 @@
           <t>Monsieur</t>
         </is>
       </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>JABIR</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>ANOUAR ZAKARIA</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>02-03-1995</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>HAY HASSANI</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>LOT LAIMOUNE VILLA  NR 117</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>BK390259</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>25-12-2030</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>Associé Gérant</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
       </c>
       <c r="U6" t="n">
-        <v>12</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>13-05-2024</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>12-05-2026</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>13-05-2024</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>3000 TTC</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ELBI LINK</t>
+          <t>FOR YOU PRO</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -855,10 +991,12 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3487719000060</v>
-      </c>
-      <c r="D7" t="n">
-        <v>100000</v>
+        <v>3519425000023</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>100 000</t>
+        </is>
       </c>
       <c r="E7" t="n">
         <v>1000</v>
@@ -875,94 +1013,100 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>15-03-2024</t>
+          <t>14-05-2024</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Monsieur</t>
+          <t>Madame</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>AZIZ</t>
+          <t>BOUNOUARIA</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>QASBAJI</t>
-        </is>
-      </c>
-      <c r="L7" t="n">
-        <v>27346</v>
+          <t>KHADIJA</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>12-06-1986</t>
+        </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>RABAT</t>
+          <t>MAARIF CASABLANCA ANFA</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>LOT ZAHRA NR 388 HAD SOUALEM BERRECHID</t>
+          <t>LISSASFA 2 BC B NO 156</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>A781595</t>
+          <t>BK503621</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>24-03-2029</t>
+          <t>28-09-2026</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
-        </is>
-      </c>
+          <t>Associée Unique Gérante</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
       </c>
       <c r="U7" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>19-03-2024</t>
+          <t>16-05-2024</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>18-03-2025</t>
+          <t>15-05-2026</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>19-03-2024</t>
-        </is>
-      </c>
+          <t>16-05-2024</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr"/>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>1000 HT</t>
-        </is>
-      </c>
+          <t>3000 TTC</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LES NOUVEAUX BATISSEURS HAOUZ</t>
+          <t>EBATRO</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3506233000023</v>
+        <v>3536486000029</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -979,12 +1123,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
+          <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>22-04-2024</t>
+          <t>10-06-2024</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -994,77 +1138,81 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>JABIR</t>
+          <t>AHMED</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>ANOUAR ZAKARIA</t>
+          <t>BARKA</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>02-03-1995</t>
+          <t>01-01-1963</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>HAY HASSANI</t>
+          <t>HAD SOUALEM BERRECHID</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>LOT LAIMOUNE VILLA  NR 117</t>
+          <t>EL ALIA 1 BD OD TANSSIFET NR 477 EL OULFA CASA</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>BK390259</t>
+          <t>WA981</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>25-12-2030</t>
+          <t>15-09-2029</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>Associé Gérant</t>
-        </is>
-      </c>
+          <t>Associé Unique Gérant</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
       </c>
       <c r="U8" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>13-05-2024</t>
+          <t>23-06-2024</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>12-05-2026</t>
+          <t>22-06-2025</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>13-05-2024</t>
-        </is>
-      </c>
+          <t>24-06-2024</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr"/>
       <c r="Z8" t="inlineStr">
         <is>
-          <t>3000 TTC</t>
-        </is>
-      </c>
+          <t>1200 HT</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>FOR YOU PRO</t>
+          <t>TRADE VENTURE</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1073,7 +1221,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3519425000023</v>
+        <v>3541348000093</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1090,92 +1238,96 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
+          <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>14-05-2024</t>
+          <t>21/06/2024</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Madame</t>
+          <t>Monsieur</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>BOUNOUARIA</t>
+          <t>RACHID</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>KHADIJA</t>
+          <t>ANAKRI</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>12-06-1986</t>
+          <t>23/04/1993</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>MAARIF CASABLANCA ANFA</t>
+          <t>AIT BAHA CHTOUKA</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>LISSASFA 2 BC B NO 156</t>
+          <t>LOT MANDAROUNA RUE 01 NR 126 AIN CHOCK CASA</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>BK503621</t>
+          <t>BK392462</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>28-09-2026</t>
+          <t>21-06-2024</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>Associée Unique Gérante</t>
-        </is>
-      </c>
+          <t>Associé Unique Gérant</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
       </c>
       <c r="U9" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>16-05-2024</t>
+          <t>29-07-2024</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>15-05-2026</t>
+          <t>28-07-2025</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>16-05-2024</t>
-        </is>
-      </c>
+          <t>29-07-2024</t>
+        </is>
+      </c>
+      <c r="Y9" t="inlineStr"/>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>3000 TTC</t>
-        </is>
-      </c>
+          <t>1200 HT</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EBATRO</t>
+          <t>BIG TOOLS</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1184,7 +1336,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3536486000029</v>
+        <v>3558967000068</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1206,7 +1358,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>10-06-2024</t>
+          <t>25-07-2024</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1216,37 +1368,37 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>AHMED</t>
+          <t>NOUREDDINE</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>BARKA</t>
+          <t>NAJMA</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>01-01-1963</t>
+          <t>16-12-1980</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>HAD SOUALEM BERRECHID</t>
+          <t>MAARIF CASABLANCA ANFA</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>EL ALIA 1 BD OD TANSSIFET NR 477 EL OULFA CASA</t>
+          <t>107 RUE MIMOUZA ETAGE 3 APP 6 HAY ERRAHA CASA</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>WA981</t>
+          <t>BE748216</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>15-09-2029</t>
+          <t>16-02-2021</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1254,6 +1406,8 @@
           <t>Associé Unique Gérant</t>
         </is>
       </c>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr">
         <is>
           <t>Casablanca</t>
@@ -1264,29 +1418,31 @@
       </c>
       <c r="V10" t="inlineStr">
         <is>
-          <t>23-06-2024</t>
+          <t>05-08-2024</t>
         </is>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>22-06-2025</t>
+          <t>04-08-2025</t>
         </is>
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>24-06-2024</t>
-        </is>
-      </c>
+          <t>05-08-2024</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr"/>
       <c r="Z10" t="inlineStr">
         <is>
-          <t>1200 HT</t>
-        </is>
-      </c>
+          <t>1500 TTC</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TRADE VENTURE</t>
+          <t>ELECTRO MJA</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1295,7 +1451,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3541348000093</v>
+        <v>3558971000057</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1317,7 +1473,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>21/06/2024</t>
+          <t>25-07-2024</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1327,37 +1483,37 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>RACHID</t>
+          <t>ABDELJALIL</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>ANAKRI</t>
+          <t>NAJMA</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>23/04/1993</t>
+          <t>21-12-1977</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>AIT BAHA CHTOUKA</t>
+          <t>MAARIF CASBLANCA ANFA</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>LOT MANDAROUNA RUE 01 NR 126 AIN CHOCK CASA</t>
+          <t>HAJ FATEH 39 APPT 9 HAY HASSANI CASA</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>BK392462</t>
+          <t>BE730556</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>21-06-2024</t>
+          <t>28-06-2020</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1365,6 +1521,8 @@
           <t>Associé Unique Gérant</t>
         </is>
       </c>
+      <c r="R11" t="inlineStr"/>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr">
         <is>
           <t>Casablanca</t>
@@ -1375,38 +1533,40 @@
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>29-07-2024</t>
+          <t>05-08-2024</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>28-07-2025</t>
+          <t>04-08-2025</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>29-07-2024</t>
-        </is>
-      </c>
+          <t>05-08-2024</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr"/>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>1200 HT</t>
-        </is>
-      </c>
+          <t>1500 TTC</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BIG TOOLS</t>
+          <t>YORA FABRIC</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3558967000068</v>
+        <v>3586789000042</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1428,7 +1588,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>25-07-2024</t>
+          <t>20-09-2024</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1438,37 +1598,37 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>NOUREDDINE</t>
+          <t>YOUSSEF</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>NAJMA</t>
+          <t>NACIRI</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>16-12-1980</t>
+          <t>25-04-1997</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>MAARIF CASABLANCA ANFA</t>
+          <t>BERRECHID</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>107 RUE MIMOUZA ETAGE 3 APP 6 HAY ERRAHA CASA</t>
+          <t>42 PASSAGE 13 HAY TISSIR 2 BERRECHID</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>BE748216</t>
+          <t>WA257624</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>16-02-2021</t>
+          <t>16-08-2029</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
@@ -1476,48 +1636,62 @@
           <t>Associé Unique Gérant</t>
         </is>
       </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>+212651652133</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>fidubasma@gmail.com</t>
+        </is>
+      </c>
       <c r="T12" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
       </c>
       <c r="U12" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="V12" t="inlineStr">
         <is>
-          <t>05-08-2024</t>
+          <t>30-09-2024</t>
         </is>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>04-08-2025</t>
+          <t>29-09-2026</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>05-08-2024</t>
-        </is>
+          <t>30-09-2024</t>
+        </is>
+      </c>
+      <c r="Y12" t="n">
+        <v>62.5</v>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>1500 TTC</t>
-        </is>
-      </c>
+          <t>3000 TTC</t>
+        </is>
+      </c>
+      <c r="AA12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ELECTRO MJA</t>
+          <t>J.M.Élégance</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3558971000057</v>
+        <v>3590885000030</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1539,7 +1713,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>25-07-2024</t>
+          <t>26-09-2024</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1549,42 +1723,52 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>ABDELJALIL</t>
+          <t>ISMAIL</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>NAJMA</t>
+          <t>JAAFAR</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>21-12-1977</t>
+          <t>15-11-1987</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>MAARIF CASBLANCA ANFA</t>
+          <t>BEN MSIK SIDI OTHMANE</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>HAJ FATEH 39 APPT 9 HAY HASSANI CASA</t>
+          <t>JAMILA 3 RUE 20 N 24 C D CASABLANCA</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>BE730556</t>
+          <t>BH443642</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>28-06-2020</t>
+          <t>18-05-2032</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
+          <t>Associé Gérant</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>‎‎+212601619808‎‎</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>dg.enswork@gmail.com</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
@@ -1597,38 +1781,42 @@
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>05-08-2024</t>
+          <t>30-09-2024</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>04-08-2025</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>05-08-2024</t>
-        </is>
+          <t>30-09-2024</t>
+        </is>
+      </c>
+      <c r="Y13" t="n">
+        <v>83.33</v>
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>1500 TTC</t>
-        </is>
-      </c>
+          <t>1000 HT</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>YORA FABRIC</t>
+          <t>VOLTI IMMO</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3586789000042</v>
+        <v>3599226000057</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1648,10 +1836,8 @@
           <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr">
-        <is>
-          <t>20-09-2024</t>
-        </is>
+      <c r="H14" t="n">
+        <v>45574</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1660,37 +1846,37 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>YOUSSEF</t>
+          <t>MOHAMED</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>NACIRI</t>
+          <t>EL BARRAK</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>25-04-1997</t>
+          <t>08-03-1987</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>BERRECHID</t>
+          <t>KSAR EL KEBIR</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>42 PASSAGE 13 HAY TISSIR 2 BERRECHID</t>
+          <t>HAY MAJOULINE DERB ROUMMAN NO 116 KSAR EL KEBIR</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>WA257624</t>
+          <t>LB125025</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>16-08-2029</t>
+          <t>11-01-2033</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
@@ -1700,7 +1886,7 @@
       </c>
       <c r="R14" t="inlineStr">
         <is>
-          <t>+212651652133</t>
+          <t>+212602853362</t>
         </is>
       </c>
       <c r="S14" t="inlineStr">
@@ -1718,17 +1904,17 @@
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>30-09-2024</t>
+          <t>11-10-2024</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>29-09-2026</t>
+          <t>10-10-2026</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>30-09-2024</t>
+          <t>11-10-2024</t>
         </is>
       </c>
       <c r="Y14" t="n">
@@ -1736,14 +1922,15 @@
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>3000 TTC</t>
-        </is>
-      </c>
+          <t>1500 TTC</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>J.M.Élégance</t>
+          <t>EXEIS Conseil</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1752,7 +1939,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3590885000030</v>
+        <v>3612832000034</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1774,7 +1961,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>26-09-2024</t>
+          <t>28-10-2024</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1784,37 +1971,37 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>ISMAIL</t>
+          <t>YOUNESS</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>JAAFAR</t>
+          <t>TABTI</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>15-11-1987</t>
+          <t>15-06-1981</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>BEN MSIK SIDI OTHMANE</t>
+          <t>SIDI BERNOUSSI</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>JAMILA 3 RUE 20 N 24 C D CASABLANCA</t>
+          <t>LOT AL BADR G 2 IMM 9 N 9 ETG 2 SD HAJJAJ OD HASSAR TIT MELLIL CASA</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>BH443642</t>
+          <t>BJ290009</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>18-05-2032</t>
+          <t>26-02-2029</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -1822,16 +2009,8 @@
           <t>Associé Gérant</t>
         </is>
       </c>
-      <c r="R15" t="inlineStr">
-        <is>
-          <t>‎‎+212601619808‎‎</t>
-        </is>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>dg.enswork@gmail.com</t>
-        </is>
-      </c>
+      <c r="R15" t="inlineStr"/>
+      <c r="S15" t="inlineStr"/>
       <c r="T15" t="inlineStr">
         <is>
           <t>Casablanca</t>
@@ -1842,17 +2021,17 @@
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>30-09-2024</t>
+          <t>30-10-2024</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>30-09-2024</t>
+          <t>30-10-2024</t>
         </is>
       </c>
       <c r="Y15" t="n">
@@ -1863,20 +2042,21 @@
           <t>1000 HT</t>
         </is>
       </c>
+      <c r="AA15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>VOLTI IMMO</t>
+          <t>AWRIMA</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3599226000057</v>
+        <v>3620039000027</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1896,8 +2076,10 @@
           <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
         </is>
       </c>
-      <c r="H16" t="n">
-        <v>45574</v>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>08-11-2024</t>
+        </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -1906,54 +2088,46 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>MOHAMED</t>
+          <t>SAAD EDDINE</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>EL BARRAK</t>
+          <t>ASARGA</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>08-03-1987</t>
+          <t>10-02-2006</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>KSAR EL KEBIR</t>
+          <t>AIN CHOCK</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>HAY MAJOULINE DERB ROUMMAN NO 116 KSAR EL KEBIR</t>
+          <t>LOT NASSIM 2 NR 34 TEG 2 SIDI MAAROUF</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>LB125025</t>
+          <t>BW56432</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>11-01-2033</t>
+          <t>31-07-2034</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
-        </is>
-      </c>
-      <c r="R16" t="inlineStr">
-        <is>
-          <t>+212602853362</t>
-        </is>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>fidubasma@gmail.com</t>
-        </is>
-      </c>
+          <t>Associé Gérant</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr"/>
+      <c r="S16" t="inlineStr"/>
       <c r="T16" t="inlineStr">
         <is>
           <t>Casablanca</t>
@@ -1964,17 +2138,17 @@
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>11-10-2024</t>
+          <t>13-11-2024</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>10-10-2026</t>
+          <t>12-11-2026</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>11-10-2024</t>
+          <t>13-11-2024</t>
         </is>
       </c>
       <c r="Y16" t="n">
@@ -1982,23 +2156,24 @@
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>1500 TTC</t>
-        </is>
-      </c>
+          <t>3000 TTC</t>
+        </is>
+      </c>
+      <c r="AA16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>EXEIS Conseil</t>
+          <t>ESTEO</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3612832000034</v>
+        <v>3647072000061</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -2020,7 +2195,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>28-10-2024</t>
+          <t>24-12-2024</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -2030,42 +2205,52 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>YOUNESS</t>
+          <t>MOHAMED</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>TABTI</t>
+          <t>ZERHOUNI</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>15-06-1981</t>
+          <t>29-09-1978</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>SIDI BERNOUSSI</t>
+          <t>AIN CHOCK</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>LOT AL BADR G 2 IMM 9 N 9 ETG 2 SD HAJJAJ OD HASSAR TIT MELLIL CASA</t>
+          <t>138 FRUE BRAHIM NAKHAI ETG 1 APT 1 MAARIF CASA</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>BJ290009</t>
+          <t>BL528</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>26-02-2029</t>
+          <t>11-07-2031</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>Associé Gérant</t>
+          <t>Associé Unique Gérant</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>+212660107020</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>contact@bociel.com</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
@@ -2074,45 +2259,46 @@
         </is>
       </c>
       <c r="U17" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>30-10-2024</t>
+          <t>01-01-2025</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>01-01-2028</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>30-10-2024</t>
+          <t>01-01-2025</t>
         </is>
       </c>
       <c r="Y17" t="n">
-        <v>83.33</v>
+        <v>75</v>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>1000 HT</t>
-        </is>
-      </c>
+          <t>2700 HT</t>
+        </is>
+      </c>
+      <c r="AA17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>AWRIMA</t>
+          <t>BIRKAN</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3620039000027</v>
+        <v>3653188000023</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -2134,7 +2320,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>08-11-2024</t>
+          <t>04-01-2025</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -2144,42 +2330,52 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>SAAD EDDINE</t>
+          <t>SOUFIANE</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>ASARGA</t>
+          <t>BENABBAD</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>10-02-2006</t>
+          <t>27-08-1990</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>AIN CHOCK</t>
+          <t>LAAOUNATE SIDI BENNOUR</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>LOT NASSIM 2 NR 34 TEG 2 SIDI MAAROUF</t>
+          <t>EL OUAFAE 1 NR 1596 KENITRA</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>BW56432</t>
+          <t>G536010</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>31-07-2034</t>
+          <t>22-06-2030</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Associé Gérant</t>
+          <t>Associé Unique Gérant</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>0661547473</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>Fidubasma@gmail.com</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
@@ -2192,32 +2388,33 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>09-01-2025</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>12-11-2026</t>
+          <t>08-01-2027</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>09-01-2025</t>
         </is>
       </c>
       <c r="Y18" t="n">
-        <v>62.5</v>
+        <v>69.44</v>
       </c>
       <c r="Z18" t="inlineStr">
         <is>
-          <t>3000 TTC</t>
-        </is>
-      </c>
+          <t>2000 TTC</t>
+        </is>
+      </c>
+      <c r="AA18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ESTEO</t>
+          <t>SALTARV</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2226,7 +2423,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3647072000061</v>
+        <v>3659240000064</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -2248,7 +2445,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>24-12-2024</t>
+          <t>11-01-2025</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2258,52 +2455,52 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>MOHAMED</t>
+          <t>SALAH</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>ZERHOUNI</t>
+          <t>MORTADA</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>29-09-1978</t>
+          <t>01-01-1982</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>AIN CHOCK</t>
+          <t>OULAD FARES SETTAT</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>138 FRUE BRAHIM NAKHAI ETG 1 APT 1 MAARIF CASA</t>
+          <t>LOT MOHANAD NR 81 LISSASFA CASABLANCA</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>BL528</t>
+          <t>WB106064</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>11-07-2031</t>
+          <t>19-11-2034</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
+          <t>Associé Gérant</t>
         </is>
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>+212660107020</t>
+          <t>0668666099</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>contact@bociel.com</t>
+          <t>fidubasma@gmail.com</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
@@ -2312,45 +2509,46 @@
         </is>
       </c>
       <c r="U19" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>01-01-2025</t>
+          <t>22-01-2025</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>01-01-2028</t>
+          <t>21-01-2027</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>01-01-2025</t>
+          <t>22-01-2025</t>
         </is>
       </c>
       <c r="Y19" t="n">
-        <v>75</v>
+        <v>69.44</v>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2700 HT</t>
-        </is>
-      </c>
+          <t>2000 TTC</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BIRKAN</t>
+          <t>ZAOUIA BUILDING</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3653188000023</v>
+        <v>3664174000027</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -2372,7 +2570,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>04-01-2025</t>
+          <t>17-01-2025</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2382,52 +2580,52 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>SOUFIANE</t>
+          <t>ABDElKRIM</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>BENABBAD</t>
+          <t>ELMORSLI</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>27-08-1990</t>
+          <t>01-01-1975</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>LAAOUNATE SIDI BENNOUR</t>
+          <t>EL JOUALA EL KELAA DES SRAGHNA</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>EL OUAFAE 1 NR 1596 KENITRA</t>
+          <t>HAY ELHANA II NR 1557 EL KELAADES SRAGHNA</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>G536010</t>
+          <t>Y145010</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>22-06-2030</t>
+          <t>07-01-2031</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
+          <t>Associé Gérant</t>
         </is>
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>0661547473</t>
+          <t>+212662611541</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>Fidubasma@gmail.com</t>
+          <t>elmorsli.a@gmail.com</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
@@ -2436,45 +2634,46 @@
         </is>
       </c>
       <c r="U20" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="V20" t="inlineStr">
         <is>
-          <t>09-01-2025</t>
+          <t>27-01-2025</t>
         </is>
       </c>
       <c r="W20" t="inlineStr">
         <is>
-          <t>08-01-2027</t>
+          <t>26-01-2026</t>
         </is>
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>09-01-2025</t>
+          <t>27-01-2025</t>
         </is>
       </c>
       <c r="Y20" t="n">
-        <v>69.44</v>
+        <v>83.33</v>
       </c>
       <c r="Z20" t="inlineStr">
         <is>
-          <t>2000 TTC</t>
-        </is>
-      </c>
+          <t>1000 HT</t>
+        </is>
+      </c>
+      <c r="AA20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SALTARV</t>
+          <t>MAMOURAN</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3659240000064</v>
+        <v>3605680000011</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -2496,7 +2695,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>11-01-2025</t>
+          <t>15-01-2025</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -2506,37 +2705,37 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>SALAH</t>
+          <t>HICHAM</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>MORTADA</t>
+          <t>SADOUK</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>01-01-1982</t>
+          <t>24-11-1971</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>OULAD FARES SETTAT</t>
+          <t>MEKNES</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>LOT MOHANAD NR 81 LISSASFA CASABLANCA</t>
+          <t>VILLA PIVOINE RUE MESK LIL SABLE D'OR HARHOURA TEMARA</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>WB106064</t>
+          <t>D329996</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>19-11-2034</t>
+          <t>24-11-2034</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -2546,12 +2745,12 @@
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>0668666099</t>
+          <t>+212600016210</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>fidubasma@gmail.com</t>
+          <t>Hicham.sadouk@persee-maroc.org</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
@@ -2560,36 +2759,37 @@
         </is>
       </c>
       <c r="U21" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>22-01-2025</t>
+          <t>27-01-2025</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>21-01-2027</t>
+          <t>26-01-2026</t>
         </is>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>22-01-2025</t>
+          <t>27-01-2025</t>
         </is>
       </c>
       <c r="Y21" t="n">
-        <v>69.44</v>
+        <v>83.33</v>
       </c>
       <c r="Z21" t="inlineStr">
         <is>
-          <t>2000 TTC</t>
-        </is>
-      </c>
+          <t>1000 HT</t>
+        </is>
+      </c>
+      <c r="AA21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ZAOUIA BUILDING</t>
+          <t>ARM Partners</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2598,7 +2798,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3664174000027</v>
+        <v>3661275000021</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -2620,7 +2820,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>17-01-2025</t>
+          <t>15-01-2025</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -2630,37 +2830,37 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>ABDElKRIM</t>
+          <t>ROCHDI</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>ELMORSLI</t>
+          <t>ALLOULI</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>01-01-1975</t>
+          <t>17-04-1978</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>EL JOUALA EL KELAA DES SRAGHNA</t>
+          <t>SIDI YOUSSEF BEN ALI MARRAKECH</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>HAY ELHANA II NR 1557 EL KELAADES SRAGHNA</t>
+          <t>LOT FAL GREEN IMM 01 ETG 03 NR 18 BOUSKOURA CASABLANCA</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Y145010</t>
+          <t>E580856</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>07-01-2031</t>
+          <t>22-03-2032</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
@@ -2670,12 +2870,12 @@
       </c>
       <c r="R22" t="inlineStr">
         <is>
-          <t>+212662611541</t>
+          <t>0661964601</t>
         </is>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>elmorsli.a@gmail.com</t>
+          <t>Rochdi.allouli@gmail.com</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
@@ -2688,17 +2888,17 @@
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>27-01-2025</t>
+          <t>28-01-2025</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>26-01-2026</t>
+          <t>27-01-2026</t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>27-01-2025</t>
+          <t>28-01-2025</t>
         </is>
       </c>
       <c r="Y22" t="n">
@@ -2709,11 +2909,12 @@
           <t>1000 HT</t>
         </is>
       </c>
+      <c r="AA22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MAMOURAN</t>
+          <t>CCGR</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2722,7 +2923,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3605680000011</v>
+        <v>3660522000079</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -2744,7 +2945,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>15-01-2025</t>
+          <t>13-01-2025</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -2754,37 +2955,37 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>HICHAM</t>
+          <t>HAJAR</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>SADOUK</t>
+          <t>FALAH</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>24-11-1971</t>
+          <t>14-05-1997</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>MEKNES</t>
+          <t>MAARIF CASABLANCA ANFA</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>VILLA PIVOINE RUE MESK LIL SABLE D'OR HARHOURA TEMARA</t>
+          <t>AIN CHOCK RUE 47 N 12 CASABLANCA</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>D329996</t>
+          <t>BK683653</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>24-11-2034</t>
+          <t>25-05-2026</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
@@ -2792,61 +2993,54 @@
           <t>Associé Gérant</t>
         </is>
       </c>
-      <c r="R23" t="inlineStr">
-        <is>
-          <t>+212600016210</t>
-        </is>
-      </c>
-      <c r="S23" t="inlineStr">
-        <is>
-          <t>Hicham.sadouk@persee-maroc.org</t>
-        </is>
-      </c>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
       <c r="T23" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
       </c>
       <c r="U23" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>27-01-2025</t>
+          <t>24-01-2025</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>26-01-2026</t>
+          <t>23-06-2027</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>27-01-2025</t>
+          <t>24-01-2025</t>
         </is>
       </c>
       <c r="Y23" t="n">
-        <v>83.33</v>
+        <v>138.88</v>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>1000 HT</t>
-        </is>
-      </c>
+          <t>2000 TTC</t>
+        </is>
+      </c>
+      <c r="AA23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>ARM Partners</t>
+          <t>NEXT GEN OFFICE</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3661275000021</v>
+        <v>3677413000019</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -2868,62 +3062,62 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>15-01-2025</t>
+          <t>04-02-2025</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Monsieur</t>
+          <t>Madame</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>ROCHDI</t>
+          <t>MEHDIA</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>ALLOULI</t>
+          <t>OUAHABI</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>17-04-1978</t>
+          <t>10-06-1985</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>SIDI YOUSSEF BEN ALI MARRAKECH</t>
+          <t>TETOUAN</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>LOT FAL GREEN IMM 01 ETG 03 NR 18 BOUSKOURA CASABLANCA</t>
+          <t>LOT GHAITA NR 41 ETG 2 CENTRE BOUSKOURA CASA</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>E580856</t>
+          <t>L419308</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>22-03-2032</t>
+          <t>27-11-2032</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>Associé Gérant</t>
+          <t>Associé Unique Gérant</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>0661964601</t>
+          <t>0701097888</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>Rochdi.allouli@gmail.com</t>
+          <t>nextgenoffice25@gmail.com</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
@@ -2936,17 +3130,17 @@
       </c>
       <c r="V24" t="inlineStr">
         <is>
-          <t>28-01-2025</t>
+          <t>05-02-2025</t>
         </is>
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>27-01-2026</t>
+          <t>04-02-2026</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
         <is>
-          <t>28-01-2025</t>
+          <t>05-02-2025</t>
         </is>
       </c>
       <c r="Y24" t="n">
@@ -2954,14 +3148,15 @@
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>1000 HT</t>
-        </is>
-      </c>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="AA24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CCGR</t>
+          <t>DOVVO DISTRIBUTION</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -2970,7 +3165,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3660522000079</v>
+        <v>3676370000050</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -2992,7 +3187,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>13-01-2025</t>
+          <t>03-02-2025</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -3002,42 +3197,52 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>HAJAR</t>
+          <t>ALI</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>FALAH</t>
+          <t>GHARBAL</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>14-05-1997</t>
+          <t>01-01-1974</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>MAARIF CASABLANCA ANFA</t>
+          <t>OULAD AMRANE SIDI BENNOUR</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>AIN CHOCK RUE 47 N 12 CASABLANCA</t>
+          <t>LOT EL WIFAK RUE 41 NR 13 AIN CHOCK CASA</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>BK683653</t>
+          <t>BK113465</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>25-05-2026</t>
+          <t>07-05-2028</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
           <t>Associé Gérant</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>0661066096</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>fidubasma@gmail.com</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
@@ -3050,17 +3255,17 @@
       </c>
       <c r="V25" t="inlineStr">
         <is>
-          <t>24-01-2025</t>
+          <t>05-02-2025</t>
         </is>
       </c>
       <c r="W25" t="inlineStr">
         <is>
-          <t>23-06-2027</t>
+          <t>04-07-2027</t>
         </is>
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>24-01-2025</t>
+          <t>05-02-2025</t>
         </is>
       </c>
       <c r="Y25" t="n">
@@ -3071,11 +3276,12 @@
           <t>2000 TTC</t>
         </is>
       </c>
+      <c r="AA25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>NEXT GEN OFFICE</t>
+          <t>SKY NEST</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3084,16 +3290,14 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3677413000019</v>
+        <v>3338405000024</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>100 000</t>
-        </is>
-      </c>
-      <c r="E26" t="n">
-        <v>1000</v>
-      </c>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="inlineStr">
         <is>
           <t>Marocaine</t>
@@ -3101,69 +3305,53 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>04-02-2025</t>
-        </is>
-      </c>
+          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°8</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Madame</t>
+          <t>Monsieur</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>MEHDIA</t>
+          <t>NAWFAL</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>OUAHABI</t>
+          <t>ADERGHAL</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>10-06-1985</t>
+          <t>29820</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>TETOUAN</t>
+          <t>Khemisset</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>LOT GHAITA NR 41 ETG 2 CENTRE BOUSKOURA CASA</t>
+          <t>Rue Addamir El Kabir Etg 04 Apt 32</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>L419308</t>
-        </is>
-      </c>
-      <c r="P26" t="inlineStr">
-        <is>
-          <t>27-11-2032</t>
-        </is>
-      </c>
+          <t>X230258</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr"/>
       <c r="Q26" t="inlineStr">
         <is>
           <t>Associé Unique Gérant</t>
         </is>
       </c>
-      <c r="R26" t="inlineStr">
-        <is>
-          <t>0701097888</t>
-        </is>
-      </c>
-      <c r="S26" t="inlineStr">
-        <is>
-          <t>nextgenoffice25@gmail.com</t>
-        </is>
-      </c>
+      <c r="R26" t="inlineStr"/>
+      <c r="S26" t="inlineStr"/>
       <c r="T26" t="inlineStr">
         <is>
           <t>Casablanca</t>
@@ -3172,52 +3360,33 @@
       <c r="U26" t="n">
         <v>12</v>
       </c>
-      <c r="V26" t="inlineStr">
-        <is>
-          <t>05-02-2025</t>
-        </is>
-      </c>
-      <c r="W26" t="inlineStr">
-        <is>
-          <t>04-02-2026</t>
-        </is>
-      </c>
-      <c r="X26" t="inlineStr">
-        <is>
-          <t>05-02-2025</t>
-        </is>
-      </c>
-      <c r="Y26" t="n">
-        <v>83.33</v>
-      </c>
-      <c r="Z26" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
+      <c r="Z26" t="inlineStr"/>
+      <c r="AA26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>DOVVO DISTRIBUTION</t>
+          <t>SABOUNI</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3676370000050</v>
+        <v>112244454</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
           <t>100 000</t>
         </is>
       </c>
-      <c r="E27" t="n">
-        <v>1000</v>
-      </c>
+      <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr">
         <is>
           <t>Marocaine</t>
@@ -3225,52 +3394,52 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
+          <t>96 BD D'ANFA ETAGE 9 APPT N° 91 RESIDENCE LE PRINTEMPS D'ANFA</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>03-02-2025</t>
+          <t>29-07-2025</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Monsieur</t>
+          <t>Madame</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>ALI</t>
+          <t>ASIRA</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>GHARBAL</t>
+          <t>ASOUDA</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>01-01-1974</t>
+          <t>14-03-2012</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>OULAD AMRANE SIDI BENNOUR</t>
+          <t>CASA</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>LOT EL WIFAK RUE 41 NR 13 AIN CHOCK CASA</t>
+          <t>DOULAKIYRTR RUE ABouALI</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>BK113465</t>
+          <t>F2259645</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>07-05-2028</t>
+          <t>26-07-2030</t>
         </is>
       </c>
       <c r="Q27" t="inlineStr">
@@ -3280,12 +3449,12 @@
       </c>
       <c r="R27" t="inlineStr">
         <is>
-          <t>0661066096</t>
+          <t>06625447485</t>
         </is>
       </c>
       <c r="S27" t="inlineStr">
         <is>
-          <t>fidubasma@gmail.com</t>
+          <t>Ali@RMAILCOM</t>
         </is>
       </c>
       <c r="T27" t="inlineStr">
@@ -3294,164 +3463,26 @@
         </is>
       </c>
       <c r="U27" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="V27" t="inlineStr">
         <is>
-          <t>05-02-2025</t>
+          <t>29-07-2025</t>
         </is>
       </c>
       <c r="W27" t="inlineStr">
         <is>
-          <t>04-07-2027</t>
+          <t>28-07-2026</t>
         </is>
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>05-02-2025</t>
-        </is>
-      </c>
-      <c r="Y27" t="n">
-        <v>138.88</v>
-      </c>
-      <c r="Z27" t="inlineStr">
-        <is>
-          <t>2000 TTC</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>SABOUNA</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>SARL AU</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>00000112244454</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>100 000</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Marocaine</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>96 BD D'ANFA ETAGE 9 APPT N° 91 RESIDENCE LE PRINTEMPS D'ANFA</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr">
-        <is>
           <t>29-07-2025</t>
         </is>
       </c>
-      <c r="I28" t="inlineStr">
-        <is>
-          <t>Madame</t>
-        </is>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>ASIRA</t>
-        </is>
-      </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>ASOUDA</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>14-03-2012</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
-          <t>CASA</t>
-        </is>
-      </c>
-      <c r="N28" t="inlineStr">
-        <is>
-          <t>DOULAKIYRTR RUE ABouALI</t>
-        </is>
-      </c>
-      <c r="O28" t="inlineStr">
-        <is>
-          <t>F2259645</t>
-        </is>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>26-07-2030</t>
-        </is>
-      </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>Associé Gérant</t>
-        </is>
-      </c>
-      <c r="R28" t="inlineStr">
-        <is>
-          <t>06625447485</t>
-        </is>
-      </c>
-      <c r="S28" t="inlineStr">
-        <is>
-          <t>Ali@RMAILCOM</t>
-        </is>
-      </c>
-      <c r="T28" t="inlineStr">
-        <is>
-          <t>Casablanca</t>
-        </is>
-      </c>
-      <c r="U28" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="V28" t="inlineStr">
-        <is>
-          <t>29-07-2025</t>
-        </is>
-      </c>
-      <c r="W28" t="inlineStr">
-        <is>
-          <t>28-07-2026</t>
-        </is>
-      </c>
-      <c r="X28" t="inlineStr">
-        <is>
-          <t>29-07-2025</t>
-        </is>
-      </c>
-      <c r="Y28" t="inlineStr">
-        <is>
-          <t>85</t>
-        </is>
-      </c>
-      <c r="Z28" t="inlineStr">
-        <is>
-          <t>2500</t>
-        </is>
-      </c>
-      <c r="AA28" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
+      <c r="Z27" t="inlineStr"/>
+      <c r="AA27" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix(forms): header placement and associes duplication; restore backward compatibility for AssocieForm; layout fixes
</commit_message>
<xml_diff>
--- a/databases/DataBase_domiciliation.xlsx
+++ b/databases/DataBase_domiciliation.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataBaseDom" sheetId="1" state="visible" r:id="rId1"/>
@@ -20,10 +19,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -40,12 +47,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -58,14 +80,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -428,9 +453,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -815,16 +840,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>LES NOUVEAUX BATISSEURS HAOUZ</t>
+          <t>FOR YOU PRO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>3506233000023</v>
+        <v>3519425000023</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -846,52 +871,52 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>22-04-2024</t>
+          <t>14-05-2024</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>Monsieur</t>
+          <t>Madame</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>JABIR</t>
+          <t>BOUNOUARIA</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>ANOUAR ZAKARIA</t>
+          <t>KHADIJA</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>02-03-1995</t>
+          <t>12-06-1986</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>HAY HASSANI</t>
+          <t>MAARIF CASABLANCA ANFA</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>LOT LAIMOUNE VILLA  NR 117</t>
+          <t>LISSASFA 2 BC B NO 156</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>BK390259</t>
+          <t>BK503621</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>25-12-2030</t>
+          <t>28-09-2026</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>Associé Gérant</t>
+          <t>Associée Unique Gérante</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
@@ -904,17 +929,17 @@
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>13-05-2024</t>
+          <t>16-05-2024</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>12-05-2026</t>
+          <t>15-05-2026</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>13-05-2024</t>
+          <t>16-05-2024</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
@@ -926,7 +951,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FOR YOU PRO</t>
+          <t>EBATRO</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -935,7 +960,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3519425000023</v>
+        <v>3536486000029</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -952,57 +977,57 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
+          <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>14-05-2024</t>
+          <t>10-06-2024</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>Madame</t>
+          <t>Monsieur</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>BOUNOUARIA</t>
+          <t>AHMED</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>KHADIJA</t>
+          <t>BARKA</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>12-06-1986</t>
+          <t>01-01-1963</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>MAARIF CASABLANCA ANFA</t>
+          <t>HAD SOUALEM BERRECHID</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>LISSASFA 2 BC B NO 156</t>
+          <t>EL ALIA 1 BD OD TANSSIFET NR 477 EL OULFA CASA</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>BK503621</t>
+          <t>WA981</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>28-09-2026</t>
+          <t>15-09-2029</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>Associée Unique Gérante</t>
+          <t>Associé Unique Gérant</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
@@ -1011,33 +1036,33 @@
         </is>
       </c>
       <c r="U7" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>16-05-2024</t>
+          <t>23-06-2024</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>15-05-2026</t>
+          <t>22-06-2025</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>16-05-2024</t>
+          <t>24-06-2024</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>3000 TTC</t>
+          <t>1200 HT</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EBATRO</t>
+          <t>TRADE VENTURE</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1046,7 +1071,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3536486000029</v>
+        <v>3541348000093</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1068,7 +1093,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>10-06-2024</t>
+          <t>21/06/2024</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -1078,37 +1103,37 @@
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>AHMED</t>
+          <t>RACHID</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>BARKA</t>
+          <t>ANAKRI</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>01-01-1963</t>
+          <t>23/04/1993</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>HAD SOUALEM BERRECHID</t>
+          <t>AIT BAHA CHTOUKA</t>
         </is>
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>EL ALIA 1 BD OD TANSSIFET NR 477 EL OULFA CASA</t>
+          <t>LOT MANDAROUNA RUE 01 NR 126 AIN CHOCK CASA</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>WA981</t>
+          <t>BK392462</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>15-09-2029</t>
+          <t>21-06-2024</t>
         </is>
       </c>
       <c r="Q8" t="inlineStr">
@@ -1126,17 +1151,17 @@
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>23-06-2024</t>
+          <t>29-07-2024</t>
         </is>
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t>22-06-2025</t>
+          <t>28-07-2025</t>
         </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>24-06-2024</t>
+          <t>29-07-2024</t>
         </is>
       </c>
       <c r="Z8" t="inlineStr">
@@ -1148,7 +1173,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>TRADE VENTURE</t>
+          <t>BIG TOOLS</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1157,7 +1182,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3541348000093</v>
+        <v>3558967000068</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1179,7 +1204,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>21/06/2024</t>
+          <t>25-07-2024</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -1189,37 +1214,37 @@
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>RACHID</t>
+          <t>NOUREDDINE</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>ANAKRI</t>
+          <t>NAJMA</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>23/04/1993</t>
+          <t>16-12-1980</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>AIT BAHA CHTOUKA</t>
+          <t>MAARIF CASABLANCA ANFA</t>
         </is>
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>LOT MANDAROUNA RUE 01 NR 126 AIN CHOCK CASA</t>
+          <t>107 RUE MIMOUZA ETAGE 3 APP 6 HAY ERRAHA CASA</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>BK392462</t>
+          <t>BE748216</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t>21-06-2024</t>
+          <t>16-02-2021</t>
         </is>
       </c>
       <c r="Q9" t="inlineStr">
@@ -1237,29 +1262,29 @@
       </c>
       <c r="V9" t="inlineStr">
         <is>
-          <t>29-07-2024</t>
+          <t>05-08-2024</t>
         </is>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>28-07-2025</t>
+          <t>04-08-2025</t>
         </is>
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>29-07-2024</t>
+          <t>05-08-2024</t>
         </is>
       </c>
       <c r="Z9" t="inlineStr">
         <is>
-          <t>1200 HT</t>
+          <t>1500 TTC</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BIG TOOLS</t>
+          <t>ELECTRO MJA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1268,7 +1293,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3558967000068</v>
+        <v>3558971000057</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1300,7 +1325,7 @@
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>NOUREDDINE</t>
+          <t>ABDELJALIL</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1310,27 +1335,27 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>16-12-1980</t>
+          <t>21-12-1977</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>MAARIF CASABLANCA ANFA</t>
+          <t>MAARIF CASBLANCA ANFA</t>
         </is>
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>107 RUE MIMOUZA ETAGE 3 APP 6 HAY ERRAHA CASA</t>
+          <t>HAJ FATEH 39 APPT 9 HAY HASSANI CASA</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>BE748216</t>
+          <t>BE730556</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>16-02-2021</t>
+          <t>28-06-2020</t>
         </is>
       </c>
       <c r="Q10" t="inlineStr">
@@ -1370,16 +1395,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ELECTRO MJA</t>
+          <t>YORA FABRIC</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3558971000057</v>
+        <v>3586789000042</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1401,7 +1426,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>25-07-2024</t>
+          <t>20-09-2024</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1411,37 +1436,37 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>ABDELJALIL</t>
+          <t>YOUSSEF</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>NAJMA</t>
+          <t>NACIRI</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>21-12-1977</t>
+          <t>25-04-1997</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>MAARIF CASBLANCA ANFA</t>
+          <t>BERRECHID</t>
         </is>
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>HAJ FATEH 39 APPT 9 HAY HASSANI CASA</t>
+          <t>42 PASSAGE 13 HAY TISSIR 2 BERRECHID</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>BE730556</t>
+          <t>WA257624</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>28-06-2020</t>
+          <t>16-08-2029</t>
         </is>
       </c>
       <c r="Q11" t="inlineStr">
@@ -1449,39 +1474,52 @@
           <t>Associé Unique Gérant</t>
         </is>
       </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>+212651652133</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>fidubasma@gmail.com</t>
+        </is>
+      </c>
       <c r="T11" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
       </c>
       <c r="U11" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>05-08-2024</t>
+          <t>30-09-2024</t>
         </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>04-08-2025</t>
+          <t>29-09-2026</t>
         </is>
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>05-08-2024</t>
-        </is>
+          <t>30-09-2024</t>
+        </is>
+      </c>
+      <c r="Y11" t="n">
+        <v>62.5</v>
       </c>
       <c r="Z11" t="inlineStr">
         <is>
-          <t>1500 TTC</t>
+          <t>3000 TTC</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>YORA FABRIC</t>
+          <t>J.M.Élégance</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1490,7 +1528,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3586789000042</v>
+        <v>3590885000030</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1512,7 +1550,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>20-09-2024</t>
+          <t>26-09-2024</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1522,52 +1560,52 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>YOUSSEF</t>
+          <t>ISMAIL</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>NACIRI</t>
+          <t>JAAFAR</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>25-04-1997</t>
+          <t>15-11-1987</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>BERRECHID</t>
+          <t>BEN MSIK SIDI OTHMANE</t>
         </is>
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>42 PASSAGE 13 HAY TISSIR 2 BERRECHID</t>
+          <t>JAMILA 3 RUE 20 N 24 C D CASABLANCA</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>WA257624</t>
+          <t>BH443642</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>16-08-2029</t>
+          <t>18-05-2032</t>
         </is>
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
+          <t>Associé Gérant</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
         <is>
-          <t>+212651652133</t>
+          <t>‎‎+212601619808‎‎</t>
         </is>
       </c>
       <c r="S12" t="inlineStr">
         <is>
-          <t>fidubasma@gmail.com</t>
+          <t>dg.enswork@gmail.com</t>
         </is>
       </c>
       <c r="T12" t="inlineStr">
@@ -1576,7 +1614,7 @@
         </is>
       </c>
       <c r="U12" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="V12" t="inlineStr">
         <is>
@@ -1585,7 +1623,7 @@
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>29-09-2026</t>
+          <t>29-09-2025</t>
         </is>
       </c>
       <c r="X12" t="inlineStr">
@@ -1594,27 +1632,27 @@
         </is>
       </c>
       <c r="Y12" t="n">
-        <v>62.5</v>
+        <v>83.33</v>
       </c>
       <c r="Z12" t="inlineStr">
         <is>
-          <t>3000 TTC</t>
+          <t>1000 HT</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>J.M.Élégance</t>
+          <t>VOLTI IMMO</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3590885000030</v>
+        <v>3599226000057</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1634,10 +1672,8 @@
           <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
         </is>
       </c>
-      <c r="H13" t="inlineStr">
-        <is>
-          <t>26-09-2024</t>
-        </is>
+      <c r="H13" t="n">
+        <v>45574</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -1646,52 +1682,52 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>ISMAIL</t>
+          <t>MOHAMED</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>JAAFAR</t>
+          <t>EL BARRAK</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>15-11-1987</t>
+          <t>08-03-1987</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>BEN MSIK SIDI OTHMANE</t>
+          <t>KSAR EL KEBIR</t>
         </is>
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>JAMILA 3 RUE 20 N 24 C D CASABLANCA</t>
+          <t>HAY MAJOULINE DERB ROUMMAN NO 116 KSAR EL KEBIR</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>BH443642</t>
+          <t>LB125025</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>18-05-2032</t>
+          <t>11-01-2033</t>
         </is>
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>Associé Gérant</t>
+          <t>Associé Unique Gérant</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
         <is>
-          <t>‎‎+212601619808‎‎</t>
+          <t>+212602853362</t>
         </is>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>dg.enswork@gmail.com</t>
+          <t>fidubasma@gmail.com</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
@@ -1700,45 +1736,45 @@
         </is>
       </c>
       <c r="U13" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="V13" t="inlineStr">
         <is>
-          <t>30-09-2024</t>
+          <t>11-10-2024</t>
         </is>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>29-09-2025</t>
+          <t>10-10-2026</t>
         </is>
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>30-09-2024</t>
+          <t>11-10-2024</t>
         </is>
       </c>
       <c r="Y13" t="n">
-        <v>83.33</v>
+        <v>62.5</v>
       </c>
       <c r="Z13" t="inlineStr">
         <is>
-          <t>1000 HT</t>
+          <t>1500 TTC</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>VOLTI IMMO</t>
+          <t>EXEIS Conseil</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3599226000057</v>
+        <v>3612832000034</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1758,8 +1794,10 @@
           <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
         </is>
       </c>
-      <c r="H14" t="n">
-        <v>45574</v>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>28-10-2024</t>
+        </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -1768,52 +1806,42 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>MOHAMED</t>
+          <t>YOUNESS</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>EL BARRAK</t>
+          <t>TABTI</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>08-03-1987</t>
+          <t>15-06-1981</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
         <is>
-          <t>KSAR EL KEBIR</t>
+          <t>SIDI BERNOUSSI</t>
         </is>
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>HAY MAJOULINE DERB ROUMMAN NO 116 KSAR EL KEBIR</t>
+          <t>LOT AL BADR G 2 IMM 9 N 9 ETG 2 SD HAJJAJ OD HASSAR TIT MELLIL CASA</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>LB125025</t>
+          <t>BJ290009</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>11-01-2033</t>
+          <t>26-02-2029</t>
         </is>
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
-        </is>
-      </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>+212602853362</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>fidubasma@gmail.com</t>
+          <t>Associé Gérant</t>
         </is>
       </c>
       <c r="T14" t="inlineStr">
@@ -1822,36 +1850,36 @@
         </is>
       </c>
       <c r="U14" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="V14" t="inlineStr">
         <is>
-          <t>11-10-2024</t>
+          <t>30-10-2024</t>
         </is>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>10-10-2026</t>
+          <t>29-10-2025</t>
         </is>
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>11-10-2024</t>
+          <t>30-10-2024</t>
         </is>
       </c>
       <c r="Y14" t="n">
-        <v>62.5</v>
+        <v>83.33</v>
       </c>
       <c r="Z14" t="inlineStr">
         <is>
-          <t>1500 TTC</t>
+          <t>1000 HT</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>EXEIS Conseil</t>
+          <t>AWRIMA</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -1860,7 +1888,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3612832000034</v>
+        <v>3620039000027</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1882,7 +1910,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>28-10-2024</t>
+          <t>08-11-2024</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1892,37 +1920,37 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>YOUNESS</t>
+          <t>SAAD EDDINE</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>TABTI</t>
+          <t>ASARGA</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>15-06-1981</t>
+          <t>10-02-2006</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
         <is>
-          <t>SIDI BERNOUSSI</t>
+          <t>AIN CHOCK</t>
         </is>
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>LOT AL BADR G 2 IMM 9 N 9 ETG 2 SD HAJJAJ OD HASSAR TIT MELLIL CASA</t>
+          <t>LOT NASSIM 2 NR 34 TEG 2 SIDI MAAROUF</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>BJ290009</t>
+          <t>BW56432</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>26-02-2029</t>
+          <t>31-07-2034</t>
         </is>
       </c>
       <c r="Q15" t="inlineStr">
@@ -1936,45 +1964,45 @@
         </is>
       </c>
       <c r="U15" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="V15" t="inlineStr">
         <is>
-          <t>30-10-2024</t>
+          <t>13-11-2024</t>
         </is>
       </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>29-10-2025</t>
+          <t>12-11-2026</t>
         </is>
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>30-10-2024</t>
+          <t>13-11-2024</t>
         </is>
       </c>
       <c r="Y15" t="n">
-        <v>83.33</v>
+        <v>62.5</v>
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>1000 HT</t>
+          <t>3000 TTC</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AWRIMA</t>
+          <t>ESTEO</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3620039000027</v>
+        <v>3647072000061</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1996,7 +2024,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>08-11-2024</t>
+          <t>24-12-2024</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -2006,17 +2034,17 @@
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>SAAD EDDINE</t>
+          <t>MOHAMED</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>ASARGA</t>
+          <t>ZERHOUNI</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>10-02-2006</t>
+          <t>29-09-1978</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -2026,22 +2054,32 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>LOT NASSIM 2 NR 34 TEG 2 SIDI MAAROUF</t>
+          <t>138 FRUE BRAHIM NAKHAI ETG 1 APT 1 MAARIF CASA</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>BW56432</t>
+          <t>BL528</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
         <is>
-          <t>31-07-2034</t>
+          <t>11-07-2031</t>
         </is>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>Associé Gérant</t>
+          <t>Associé Unique Gérant</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>+212660107020</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>contact@bociel.com</t>
         </is>
       </c>
       <c r="T16" t="inlineStr">
@@ -2050,36 +2088,36 @@
         </is>
       </c>
       <c r="U16" t="n">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>01-01-2025</t>
         </is>
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>12-11-2026</t>
+          <t>01-01-2028</t>
         </is>
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>13-11-2024</t>
+          <t>01-01-2025</t>
         </is>
       </c>
       <c r="Y16" t="n">
-        <v>62.5</v>
+        <v>75</v>
       </c>
       <c r="Z16" t="inlineStr">
         <is>
-          <t>3000 TTC</t>
+          <t>2700 HT</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ESTEO</t>
+          <t>BIRKAN</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -2088,7 +2126,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3647072000061</v>
+        <v>3653188000023</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -2110,7 +2148,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>24-12-2024</t>
+          <t>04-01-2025</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -2120,37 +2158,37 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>MOHAMED</t>
+          <t>SOUFIANE</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>ZERHOUNI</t>
+          <t>BENABBAD</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>29-09-1978</t>
+          <t>27-08-1990</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
         <is>
-          <t>AIN CHOCK</t>
+          <t>LAAOUNATE SIDI BENNOUR</t>
         </is>
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>138 FRUE BRAHIM NAKHAI ETG 1 APT 1 MAARIF CASA</t>
+          <t>EL OUAFAE 1 NR 1596 KENITRA</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>BL528</t>
+          <t>G536010</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>11-07-2031</t>
+          <t>22-06-2030</t>
         </is>
       </c>
       <c r="Q17" t="inlineStr">
@@ -2160,12 +2198,12 @@
       </c>
       <c r="R17" t="inlineStr">
         <is>
-          <t>+212660107020</t>
+          <t>0661547473</t>
         </is>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>contact@bociel.com</t>
+          <t>Fidubasma@gmail.com</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
@@ -2174,36 +2212,36 @@
         </is>
       </c>
       <c r="U17" t="n">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="V17" t="inlineStr">
         <is>
-          <t>01-01-2025</t>
+          <t>09-01-2025</t>
         </is>
       </c>
       <c r="W17" t="inlineStr">
         <is>
-          <t>01-01-2028</t>
+          <t>08-01-2027</t>
         </is>
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>01-01-2025</t>
+          <t>09-01-2025</t>
         </is>
       </c>
       <c r="Y17" t="n">
-        <v>75</v>
+        <v>69.44</v>
       </c>
       <c r="Z17" t="inlineStr">
         <is>
-          <t>2700 HT</t>
+          <t>2000 TTC</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BIRKAN</t>
+          <t>SALTARV</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -2212,7 +2250,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>3653188000023</v>
+        <v>3659240000064</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -2234,7 +2272,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>04-01-2025</t>
+          <t>11-01-2025</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
@@ -2244,52 +2282,52 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>SOUFIANE</t>
+          <t>SALAH</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>BENABBAD</t>
+          <t>MORTADA</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>27-08-1990</t>
+          <t>01-01-1982</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
         <is>
-          <t>LAAOUNATE SIDI BENNOUR</t>
+          <t>OULAD FARES SETTAT</t>
         </is>
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>EL OUAFAE 1 NR 1596 KENITRA</t>
+          <t>LOT MOHANAD NR 81 LISSASFA CASABLANCA</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>G536010</t>
+          <t>WB106064</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>22-06-2030</t>
+          <t>19-11-2034</t>
         </is>
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
+          <t>Associé Gérant</t>
         </is>
       </c>
       <c r="R18" t="inlineStr">
         <is>
-          <t>0661547473</t>
+          <t>0668666099</t>
         </is>
       </c>
       <c r="S18" t="inlineStr">
         <is>
-          <t>Fidubasma@gmail.com</t>
+          <t>fidubasma@gmail.com</t>
         </is>
       </c>
       <c r="T18" t="inlineStr">
@@ -2302,17 +2340,17 @@
       </c>
       <c r="V18" t="inlineStr">
         <is>
-          <t>09-01-2025</t>
+          <t>22-01-2025</t>
         </is>
       </c>
       <c r="W18" t="inlineStr">
         <is>
-          <t>08-01-2027</t>
+          <t>21-01-2027</t>
         </is>
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>09-01-2025</t>
+          <t>22-01-2025</t>
         </is>
       </c>
       <c r="Y18" t="n">
@@ -2327,16 +2365,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SALTARV</t>
+          <t>ZAOUIA BUILDING</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3659240000064</v>
+        <v>3664174000027</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -2358,7 +2396,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>11-01-2025</t>
+          <t>17-01-2025</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -2368,37 +2406,37 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>SALAH</t>
+          <t>ABDElKRIM</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>MORTADA</t>
+          <t>ELMORSLI</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>01-01-1982</t>
+          <t>01-01-1975</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
         <is>
-          <t>OULAD FARES SETTAT</t>
+          <t>EL JOUALA EL KELAA DES SRAGHNA</t>
         </is>
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>LOT MOHANAD NR 81 LISSASFA CASABLANCA</t>
+          <t>HAY ELHANA II NR 1557 EL KELAADES SRAGHNA</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>WB106064</t>
+          <t>Y145010</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>19-11-2034</t>
+          <t>07-01-2031</t>
         </is>
       </c>
       <c r="Q19" t="inlineStr">
@@ -2408,12 +2446,12 @@
       </c>
       <c r="R19" t="inlineStr">
         <is>
-          <t>0668666099</t>
+          <t>+212662611541</t>
         </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>fidubasma@gmail.com</t>
+          <t>elmorsli.a@gmail.com</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
@@ -2422,36 +2460,36 @@
         </is>
       </c>
       <c r="U19" t="n">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="V19" t="inlineStr">
         <is>
-          <t>22-01-2025</t>
+          <t>27-01-2025</t>
         </is>
       </c>
       <c r="W19" t="inlineStr">
         <is>
-          <t>21-01-2027</t>
+          <t>26-01-2026</t>
         </is>
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>22-01-2025</t>
+          <t>27-01-2025</t>
         </is>
       </c>
       <c r="Y19" t="n">
-        <v>69.44</v>
+        <v>83.33</v>
       </c>
       <c r="Z19" t="inlineStr">
         <is>
-          <t>2000 TTC</t>
+          <t>1000 HT</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>ZAOUIA BUILDING</t>
+          <t>MAMOURAN</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -2460,7 +2498,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3664174000027</v>
+        <v>3605680000011</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -2482,7 +2520,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>17-01-2025</t>
+          <t>15-01-2025</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -2492,37 +2530,37 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>ABDElKRIM</t>
+          <t>HICHAM</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>ELMORSLI</t>
+          <t>SADOUK</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>01-01-1975</t>
+          <t>24-11-1971</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
         <is>
-          <t>EL JOUALA EL KELAA DES SRAGHNA</t>
+          <t>MEKNES</t>
         </is>
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>HAY ELHANA II NR 1557 EL KELAADES SRAGHNA</t>
+          <t>VILLA PIVOINE RUE MESK LIL SABLE D'OR HARHOURA TEMARA</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Y145010</t>
+          <t>D329996</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>07-01-2031</t>
+          <t>24-11-2034</t>
         </is>
       </c>
       <c r="Q20" t="inlineStr">
@@ -2532,12 +2570,12 @@
       </c>
       <c r="R20" t="inlineStr">
         <is>
-          <t>+212662611541</t>
+          <t>+212600016210</t>
         </is>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>elmorsli.a@gmail.com</t>
+          <t>Hicham.sadouk@persee-maroc.org</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
@@ -2575,7 +2613,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MAMOURAN</t>
+          <t>ARM Partners</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -2584,7 +2622,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3605680000011</v>
+        <v>3661275000021</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -2616,37 +2654,37 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>HICHAM</t>
+          <t>ROCHDI</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>SADOUK</t>
+          <t>ALLOULI</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>24-11-1971</t>
+          <t>17-04-1978</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
         <is>
-          <t>MEKNES</t>
+          <t>SIDI YOUSSEF BEN ALI MARRAKECH</t>
         </is>
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>VILLA PIVOINE RUE MESK LIL SABLE D'OR HARHOURA TEMARA</t>
+          <t>LOT FAL GREEN IMM 01 ETG 03 NR 18 BOUSKOURA CASABLANCA</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>D329996</t>
+          <t>E580856</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>24-11-2034</t>
+          <t>22-03-2032</t>
         </is>
       </c>
       <c r="Q21" t="inlineStr">
@@ -2656,12 +2694,12 @@
       </c>
       <c r="R21" t="inlineStr">
         <is>
-          <t>+212600016210</t>
+          <t>0661964601</t>
         </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
-          <t>Hicham.sadouk@persee-maroc.org</t>
+          <t>Rochdi.allouli@gmail.com</t>
         </is>
       </c>
       <c r="T21" t="inlineStr">
@@ -2674,17 +2712,17 @@
       </c>
       <c r="V21" t="inlineStr">
         <is>
-          <t>27-01-2025</t>
+          <t>28-01-2025</t>
         </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>26-01-2026</t>
+          <t>27-01-2026</t>
         </is>
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>27-01-2025</t>
+          <t>28-01-2025</t>
         </is>
       </c>
       <c r="Y21" t="n">
@@ -2699,7 +2737,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>ARM Partners</t>
+          <t>CCGR</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2708,7 +2746,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3661275000021</v>
+        <v>3660522000079</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -2730,7 +2768,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>15-01-2025</t>
+          <t>13-01-2025</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -2740,37 +2778,37 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>ROCHDI</t>
+          <t>HAJAR</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>ALLOULI</t>
+          <t>FALAH</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>17-04-1978</t>
+          <t>14-05-1997</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>SIDI YOUSSEF BEN ALI MARRAKECH</t>
+          <t>MAARIF CASABLANCA ANFA</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>LOT FAL GREEN IMM 01 ETG 03 NR 18 BOUSKOURA CASABLANCA</t>
+          <t>AIN CHOCK RUE 47 N 12 CASABLANCA</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>E580856</t>
+          <t>BK683653</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>22-03-2032</t>
+          <t>25-05-2026</t>
         </is>
       </c>
       <c r="Q22" t="inlineStr">
@@ -2778,61 +2816,51 @@
           <t>Associé Gérant</t>
         </is>
       </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>0661964601</t>
-        </is>
-      </c>
-      <c r="S22" t="inlineStr">
-        <is>
-          <t>Rochdi.allouli@gmail.com</t>
-        </is>
-      </c>
       <c r="T22" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
       </c>
       <c r="U22" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="V22" t="inlineStr">
         <is>
-          <t>28-01-2025</t>
+          <t>24-01-2025</t>
         </is>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>27-01-2026</t>
+          <t>23-06-2027</t>
         </is>
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>28-01-2025</t>
+          <t>24-01-2025</t>
         </is>
       </c>
       <c r="Y22" t="n">
-        <v>83.33</v>
+        <v>138.88</v>
       </c>
       <c r="Z22" t="inlineStr">
         <is>
-          <t>1000 HT</t>
+          <t>2000 TTC</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CCGR</t>
+          <t>NEXT GEN OFFICE</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3660522000079</v>
+        <v>3677413000019</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -2854,52 +2882,62 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>13-01-2025</t>
+          <t>04-02-2025</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Monsieur</t>
+          <t>Madame</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>HAJAR</t>
+          <t>MEHDIA</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>FALAH</t>
+          <t>OUAHABI</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>14-05-1997</t>
+          <t>10-06-1985</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>MAARIF CASABLANCA ANFA</t>
+          <t>TETOUAN</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>AIN CHOCK RUE 47 N 12 CASABLANCA</t>
+          <t>LOT GHAITA NR 41 ETG 2 CENTRE BOUSKOURA CASA</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>BK683653</t>
+          <t>L419308</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>25-05-2026</t>
+          <t>27-11-2032</t>
         </is>
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>Associé Gérant</t>
+          <t>Associé Unique Gérant</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>0701097888</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>nextgenoffice25@gmail.com</t>
         </is>
       </c>
       <c r="T23" t="inlineStr">
@@ -2908,45 +2946,45 @@
         </is>
       </c>
       <c r="U23" t="n">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="V23" t="inlineStr">
         <is>
-          <t>24-01-2025</t>
+          <t>05-02-2025</t>
         </is>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>23-06-2027</t>
+          <t>04-02-2026</t>
         </is>
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>24-01-2025</t>
+          <t>05-02-2025</t>
         </is>
       </c>
       <c r="Y23" t="n">
-        <v>138.88</v>
+        <v>83.33</v>
       </c>
       <c r="Z23" t="inlineStr">
         <is>
-          <t>2000 TTC</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>NEXT GEN OFFICE</t>
+          <t>DOVVO DISTRIBUTION</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>SARL AU</t>
+          <t>SARL</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3677413000019</v>
+        <v>3676370000050</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -2968,62 +3006,62 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>04-02-2025</t>
+          <t>03-02-2025</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Madame</t>
+          <t>Monsieur</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>MEHDIA</t>
+          <t>ALI</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>OUAHABI</t>
+          <t>GHARBAL</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>10-06-1985</t>
+          <t>01-01-1974</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>TETOUAN</t>
+          <t>OULAD AMRANE SIDI BENNOUR</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>LOT GHAITA NR 41 ETG 2 CENTRE BOUSKOURA CASA</t>
+          <t>LOT EL WIFAK RUE 41 NR 13 AIN CHOCK CASA</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>L419308</t>
+          <t>BK113465</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>27-11-2032</t>
+          <t>07-05-2028</t>
         </is>
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
+          <t>Associé Gérant</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
         <is>
-          <t>0701097888</t>
+          <t>0661066096</t>
         </is>
       </c>
       <c r="S24" t="inlineStr">
         <is>
-          <t>nextgenoffice25@gmail.com</t>
+          <t>fidubasma@gmail.com</t>
         </is>
       </c>
       <c r="T24" t="inlineStr">
@@ -3032,7 +3070,7 @@
         </is>
       </c>
       <c r="U24" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="V24" t="inlineStr">
         <is>
@@ -3041,7 +3079,7 @@
       </c>
       <c r="W24" t="inlineStr">
         <is>
-          <t>04-02-2026</t>
+          <t>04-07-2027</t>
         </is>
       </c>
       <c r="X24" t="inlineStr">
@@ -3050,35 +3088,32 @@
         </is>
       </c>
       <c r="Y24" t="n">
-        <v>83.33</v>
+        <v>138.88</v>
       </c>
       <c r="Z24" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>2000 TTC</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DOVVO DISTRIBUTION</t>
+          <t>SKY NEST</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SARL</t>
+          <t>SARL AU</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3676370000050</v>
+        <v>3338405000024</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>100 000</t>
-        </is>
-      </c>
-      <c r="E25" t="n">
-        <v>1000</v>
+          <t>100000</t>
+        </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -3087,12 +3122,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Bd Zerktouni Et Angle Rue Ibn Al Moualim N° 4, Etage 2, Appt N°10</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr">
-        <is>
-          <t>03-02-2025</t>
+          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°8</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -3102,52 +3132,37 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>ALI</t>
+          <t>NAWFAL</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>GHARBAL</t>
+          <t>ADERGHAL</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>01-01-1974</t>
+          <t>29820</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>OULAD AMRANE SIDI BENNOUR</t>
+          <t>Khemisset</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>LOT EL WIFAK RUE 41 NR 13 AIN CHOCK CASA</t>
+          <t>Rue Addamir El Kabir Etg 04 Apt 32</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>BK113465</t>
-        </is>
-      </c>
-      <c r="P25" t="inlineStr">
-        <is>
-          <t>07-05-2028</t>
+          <t>X230258</t>
         </is>
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>Associé Gérant</t>
-        </is>
-      </c>
-      <c r="R25" t="inlineStr">
-        <is>
-          <t>0661066096</t>
-        </is>
-      </c>
-      <c r="S25" t="inlineStr">
-        <is>
-          <t>fidubasma@gmail.com</t>
+          <t>Associé Unique Gérant</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
@@ -3156,36 +3171,13 @@
         </is>
       </c>
       <c r="U25" t="n">
-        <v>30</v>
-      </c>
-      <c r="V25" t="inlineStr">
-        <is>
-          <t>05-02-2025</t>
-        </is>
-      </c>
-      <c r="W25" t="inlineStr">
-        <is>
-          <t>04-07-2027</t>
-        </is>
-      </c>
-      <c r="X25" t="inlineStr">
-        <is>
-          <t>05-02-2025</t>
-        </is>
-      </c>
-      <c r="Y25" t="n">
-        <v>138.88</v>
-      </c>
-      <c r="Z25" t="inlineStr">
-        <is>
-          <t>2000 TTC</t>
-        </is>
+        <v>12</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>SKY NEST</t>
+          <t>SABOUNI</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -3194,11 +3186,11 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3338405000024</v>
+        <v>112244454</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>100000</t>
+          <t>100 000</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -3208,47 +3200,67 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Angle Bd Zerktouni Et Rue Ibn Al Moualim N° 4, Etage 2, Appt N°8</t>
+          <t>96 BD D'ANFA ETAGE 9 APPT N° 91 RESIDENCE LE PRINTEMPS D'ANFA</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>29-07-2025</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Monsieur</t>
+          <t>Madame</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>NAWFAL</t>
+          <t>ASIRA</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>ADERGHAL</t>
+          <t>ASOUDA</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>29820</t>
+          <t>14-03-2012</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>Khemisset</t>
+          <t>CASA</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>Rue Addamir El Kabir Etg 04 Apt 32</t>
+          <t>DOULAKIYRTR RUE ABouALI</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>X230258</t>
+          <t>F2259645</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>26-07-2030</t>
         </is>
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>Associé Unique Gérant</t>
+          <t>Associé Gérant</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>06625447485</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>Ali@RMAILCOM</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
@@ -3259,122 +3271,24 @@
       <c r="U26" t="n">
         <v>12</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>SABOUNI</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>SARL AU</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>112244454</v>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>100 000</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Marocaine</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>96 BD D'ANFA ETAGE 9 APPT N° 91 RESIDENCE LE PRINTEMPS D'ANFA</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr">
+      <c r="V26" t="inlineStr">
         <is>
           <t>29-07-2025</t>
         </is>
       </c>
-      <c r="I27" t="inlineStr">
-        <is>
-          <t>Madame</t>
-        </is>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>ASIRA</t>
-        </is>
-      </c>
-      <c r="K27" t="inlineStr">
-        <is>
-          <t>ASOUDA</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>14-03-2012</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
-          <t>CASA</t>
-        </is>
-      </c>
-      <c r="N27" t="inlineStr">
-        <is>
-          <t>DOULAKIYRTR RUE ABouALI</t>
-        </is>
-      </c>
-      <c r="O27" t="inlineStr">
-        <is>
-          <t>F2259645</t>
-        </is>
-      </c>
-      <c r="P27" t="inlineStr">
-        <is>
-          <t>26-07-2030</t>
-        </is>
-      </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>Associé Gérant</t>
-        </is>
-      </c>
-      <c r="R27" t="inlineStr">
-        <is>
-          <t>06625447485</t>
-        </is>
-      </c>
-      <c r="S27" t="inlineStr">
-        <is>
-          <t>Ali@RMAILCOM</t>
-        </is>
-      </c>
-      <c r="T27" t="inlineStr">
-        <is>
-          <t>Casablanca</t>
-        </is>
-      </c>
-      <c r="U27" t="n">
-        <v>12</v>
-      </c>
-      <c r="V27" t="inlineStr">
-        <is>
-          <t>29-07-2025</t>
-        </is>
-      </c>
-      <c r="W27" t="inlineStr">
+      <c r="W26" t="inlineStr">
         <is>
           <t>28-07-2026</t>
         </is>
       </c>
-      <c r="X27" t="inlineStr">
+      <c r="X26" t="inlineStr">
         <is>
           <t>29-07-2025</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3384,7 +3298,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3393,98 +3307,68 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>DEN_STE</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>FORME_JUR</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ICE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>DATE_ICE</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>CAPITAL</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>PART_SOCIAL</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>STE_ADRESS</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>TRIBUNAL</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>ACTIVITY1</t>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>denomination</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>forme_juridique</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>ice</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>date_ice</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>capital</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>parts_social</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>adresse</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>tribunal</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t>activites</t>
         </is>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>SAOUZ</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>SARL AU</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>26-09-2025</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>100 000</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>46 BD ZERKTOUNI ETG 2 APPT 6 CASABLANCA</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Casablanca</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Travaux Divers ou de Construction</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>Marchand effectuant Import Export</t>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20/10/2025</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -3508,7 +3392,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>societe_id</t>
         </is>
@@ -3525,7 +3409,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3534,69 +3418,44 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>DATE_CONTRAT</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>PERIOD_DOMCIL</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PRIX_CONTRAT</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PRIX_INTERMEDIARE_CONTRAT</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>DOM_DATEDEB</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>DOM_DATEFIN</t>
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>date_contrat</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>period</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>prix_mensuel</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>prix_inter</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>date_debut</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>date_fin</t>
         </is>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>22-09-2025</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>58</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1200</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>22-09-2025</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>28-09-2026</t>
-        </is>
-      </c>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
chore: finalize theme refactor and add style report
</commit_message>
<xml_diff>
--- a/databases/DataBase_domiciliation.xlsx
+++ b/databases/DataBase_domiciliation.xlsx
@@ -3298,7 +3298,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3354,21 +3354,49 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>20/10/2025</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr">
         <is>
           <t>[]</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SMALLL</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>SARL AU</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>20/10/2025</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>56  BOULEVARD MOULAY YOUSSEF 3EME ETAGE APPT 14, CASABLANCA</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Casablanca</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>['Travaux Divers ou de Construction', 'Marchand effectuant Import Export']</t>
         </is>
       </c>
     </row>
@@ -3383,7 +3411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3395,6 +3423,72 @@
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>societe_id</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>20/10/2025</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>20/10/2025</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>SMALLL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>20/10/2025</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>20/10/2025</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>SMALLL</t>
         </is>
       </c>
     </row>
@@ -3409,7 +3503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3449,13 +3543,14 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr"/>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
+    <row r="2"/>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix(docgen): add alias keys for associe fields and contract date to improve template matching
</commit_message>
<xml_diff>
--- a/databases/DataBase_domiciliation.xlsx
+++ b/databases/DataBase_domiciliation.xlsx
@@ -3328,7 +3328,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3698,8 +3698,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>9</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -3711,25 +3713,70 @@
           <t>SARL AU</t>
         </is>
       </c>
-      <c r="E9" s="4" t="n">
+      <c r="E9" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>10 000</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>46 BD ZERKTOUNI ETG 2 APPT 6 CASABLANCA</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Casablanca</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>FIRST BUILD</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SARL AU</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>00000125465610225</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="n">
         <v>45958</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>10 000</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>46 BD ZERKTOUNI ETG 2 APPT 6 CASABLANCA</t>
-        </is>
-      </c>
-      <c r="I9" t="inlineStr">
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>86 Ha CASABLANCA</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
@@ -3746,7 +3793,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4274,11 +4321,15 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" t="n">
-        <v>9</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -4291,16 +4342,97 @@
         </is>
       </c>
       <c r="I9" s="4" t="n"/>
-      <c r="N9" t="n">
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Associé Gérant</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>M.</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>SAWAB</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Alim</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Marocaine</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>G54887</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>10/01/2029</t>
+        </is>
+      </c>
+      <c r="I10" s="4" t="n">
+        <v>44177</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>DOUR SALIM</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>Soualem HAi Ajax Willam</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>0661545632</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>Zaimm@gmail.com</t>
+        </is>
+      </c>
+      <c r="N10" t="n">
         <v>1000</v>
       </c>
-      <c r="O9" t="n">
+      <c r="O10" t="n">
         <v>100000</v>
       </c>
-      <c r="P9" t="n">
+      <c r="P10" t="n">
         <v>1</v>
       </c>
-      <c r="Q9" t="inlineStr">
+      <c r="Q10" t="inlineStr">
         <is>
           <t>Associé Gérant</t>
         </is>
@@ -4317,7 +4449,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4560,25 +4692,63 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>9</v>
-      </c>
-      <c r="B9" t="n">
-        <v>9</v>
-      </c>
-      <c r="C9" s="4" t="n">
-        <v>45960</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="C9" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-30 00:00:00</t>
+        </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
           <t>12</t>
         </is>
       </c>
-      <c r="G9" s="4" t="n">
-        <v>45960</v>
-      </c>
-      <c r="H9" s="4" t="n">
-        <v>46325</v>
+      <c r="G9" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-30 00:00:00</t>
+        </is>
+      </c>
+      <c r="H9" s="4" t="inlineStr">
+        <is>
+          <t>2026-10-30 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>10</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>45958</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>800</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1500</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <v>45958</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>46415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore(docgen): name JSON report like HTML, remove legacy file; consolidate save UI message; expose ACTIVITY1..6 and DATE_CONTRAT in context
</commit_message>
<xml_diff>
--- a/databases/DataBase_domiciliation.xlsx
+++ b/databases/DataBase_domiciliation.xlsx
@@ -3328,7 +3328,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3740,8 +3740,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>10</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -3758,25 +3760,112 @@
           <t>00000125465610225</t>
         </is>
       </c>
-      <c r="E10" s="4" t="n">
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>10 000</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>86 Ha CASABLANCA</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Casablanca</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>ABIOP</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>SA</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>000001225200255201</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>100 000</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>N 15 Imtihane Rue 26 Rabat</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Rabat</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ASTRAPIA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SARL AU</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="n">
         <v>45958</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>10 000</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="G12" t="inlineStr">
         <is>
           <t>100</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>86 Ha CASABLANCA</t>
-        </is>
-      </c>
-      <c r="I10" t="inlineStr">
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>46 BD ZERKTOUNI ETG 2 APPT 6 CASABLANCA</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
         <is>
           <t>Casablanca</t>
         </is>
@@ -3793,7 +3882,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q10"/>
+  <dimension ref="A1:Q12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4364,11 +4453,15 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>10</v>
-      </c>
-      <c r="B10" t="n">
-        <v>10</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -4400,8 +4493,10 @@
           <t>10/01/2029</t>
         </is>
       </c>
-      <c r="I10" s="4" t="n">
-        <v>44177</v>
+      <c r="I10" s="4" t="inlineStr">
+        <is>
+          <t>2020-12-12 00:00:00</t>
+        </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -4423,16 +4518,142 @@
           <t>Zaimm@gmail.com</t>
         </is>
       </c>
-      <c r="N10" t="n">
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Associé Gérant</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Mme</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>NAIMA</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>SDIOUT</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Marocaine</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>MP155854</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>10/11/2023</t>
+        </is>
+      </c>
+      <c r="I11" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-12 00:00:00</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>BEN GURIR</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>SOULTANA OMAN FOUG SALK LIBYA</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>+212668788112</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>ANABIKOI@HOULIMA.MA</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>100000</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Associé</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>12</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>M.</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Marocaine</t>
+        </is>
+      </c>
+      <c r="I12" s="4" t="n"/>
+      <c r="N12" t="n">
         <v>1000</v>
       </c>
-      <c r="O10" t="n">
+      <c r="O12" t="n">
         <v>100000</v>
       </c>
-      <c r="P10" t="n">
+      <c r="P12" t="n">
         <v>1</v>
       </c>
-      <c r="Q10" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>Associé Gérant</t>
         </is>
@@ -4449,7 +4670,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4724,31 +4945,109 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>10</v>
-      </c>
-      <c r="B10" t="n">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="n">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="C10" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>800</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="G10" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="H10" s="4" t="inlineStr">
+        <is>
+          <t>2027-01-28 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="C11" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>81</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="G11" s="4" t="inlineStr">
+        <is>
+          <t>2025-10-28 00:00:00</t>
+        </is>
+      </c>
+      <c r="H11" s="4" t="inlineStr">
+        <is>
+          <t>2027-10-28 00:00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>12</v>
+      </c>
+      <c r="C12" s="4" t="n">
         <v>45958</v>
       </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>800</v>
-      </c>
-      <c r="F10" t="n">
-        <v>1500</v>
-      </c>
-      <c r="G10" s="4" t="n">
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="G12" s="4" t="n">
         <v>45958</v>
       </c>
-      <c r="H10" s="4" t="n">
-        <v>46415</v>
+      <c r="H12" s="4" t="n">
+        <v>45958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>